<commit_message>
ajout des excel 'templateIndividu" et "templateIndividuBis"
</commit_message>
<xml_diff>
--- a/template and fill excel/templateIndividu.xlsx
+++ b/template and fill excel/templateIndividu.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\simon\ucl\Mémoire\Gitub_Memoire\Memoire\script\template Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\simon\ucl\Mémoire\Gitub_Memoire\Memoire\template and fill excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39BFDEB4-CB4C-407C-B1DE-6C8BB32EB174}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6F680B0-AF4B-48BC-868B-E84917ED0211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A958B0B2-CF34-420D-B00A-46088B9BF900}"/>
+    <workbookView xWindow="1800" yWindow="1215" windowWidth="27000" windowHeight="14235" xr2:uid="{A958B0B2-CF34-420D-B00A-46088B9BF900}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Continent</t>
   </si>
@@ -108,6 +108,18 @@
   </si>
   <si>
     <t>SpecimenCode</t>
+  </si>
+  <si>
+    <t>Locality</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Collection_Date</t>
+  </si>
+  <si>
+    <t>Sexe</t>
   </si>
 </sst>
 </file>
@@ -485,84 +497,98 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8FC3573-E068-433B-AD5B-DE777D3635B5}">
-  <dimension ref="A1:X1"/>
+  <dimension ref="A1:AB1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="Z23" sqref="Z23"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="P1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="O1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>2</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>21</v>
       </c>
       <c r="X1" s="1" t="s">
         <v>22</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>